<commit_message>
add sentiment analysis to Explorer
</commit_message>
<xml_diff>
--- a/QCA-AID-Explorer-Config.xlsx
+++ b/QCA-AID-Explorer-Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_AD4DB114E441178AC67DF462BE53C4D2693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC482634-C115-45A1-A060-F23267189B90}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="11_AD4DB114E441178AC67DF462BE53C4D2693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D4A80CB-83AD-4C42-80D2-ECAA3E2E3B84}"/>
   <bookViews>
-    <workbookView xWindow="-4358" yWindow="8002" windowWidth="21796" windowHeight="13875" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Zusammenfassung1" sheetId="4" r:id="rId4"/>
     <sheet name="Begründungsanalyse" sheetId="5" r:id="rId5"/>
     <sheet name="BenutzerdefinierteAnalyse" sheetId="6" r:id="rId6"/>
+    <sheet name="Sentiment1" sheetId="7" r:id="rId7"/>
+    <sheet name="Sentiment2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>Parameter</t>
   </si>
@@ -219,6 +221,87 @@
   </si>
   <si>
     <t>Auszuwertende Spalte, Standard "Begründung"</t>
+  </si>
+  <si>
+    <t>sentiment_analysis</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Positiv, Negativ, Neutral</t>
+  </si>
+  <si>
+    <t>{"Positiv": "#4CAF50", "Negativ": "#F44336", "Neutral": "#9E9E9E"}</t>
+  </si>
+  <si>
+    <t>Sentiment-Analyse: Akteure (Positiv/Negativ)</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>crosstab_dimensions</t>
+  </si>
+  <si>
+    <t>Dokument, Hauptkategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figsize </t>
+  </si>
+  <si>
+    <t>12x8</t>
+  </si>
+  <si>
+    <t>Dimensionen der Grafik</t>
+  </si>
+  <si>
+    <t>14x10</t>
+  </si>
+  <si>
+    <t>Kritisch, Befürwortend, Ambivalent, Neutral</t>
+  </si>
+  <si>
+    <t>Sentiment-Analyse: Ressourcen (Kritisch/Befürwortend)</t>
+  </si>
+  <si>
+    <t>Custom Prompt</t>
+  </si>
+  <si>
+    <t>Auszuwertende Spalte</t>
+  </si>
+  <si>
+    <t>Auszuwertende Spalte, Standard "Text"</t>
+  </si>
+  <si>
+    <t>{"Kritisch": "#FF5722", "Befürwortend": "#2196F3", "Ambivalent": "#9C27B0", "Neutral": "#9E9E9E"}</t>
+  </si>
+  <si>
+    <t>sentiment_categories</t>
+  </si>
+  <si>
+    <t>color_mapping</t>
+  </si>
+  <si>
+    <t>chart_title</t>
+  </si>
+  <si>
+    <t>Du bist ein Experte für qualitative Textanalyse.
+Klassifiziere den folgenden Text in Bezug auf Ressourcen anhand des Sentiments in eine der folgenden Kategorien: Kritisch, Befürwortend, Ambivalent, Neutral
+Beachte bei deiner Analyse:
+1. Die Bewertung von Ressourcen im Text
+2. Die Tonalität gegenüber Ressourcenverfügbarkeit und -nutzung
+3. Die impliziten und expliziten Wertungen
+Text:
+---
+[Text kommt hier]
+---
+Antworte mit einem JSON-Objekt im folgenden Format:
+{
+    "sentiment": "Kategorie", // Eine der vorgegebenen Kategorien
+    "keywords": ["wort1", "wort2", "wort3"], // 3-5 Schlüsselwörter, die zur Bewertung von Ressourcen im Text entscheidend sind
+    "explanation": "Kurze Begründung" // Kurze Erklärung (1-2 Sätze)
+}</t>
   </si>
 </sst>
 </file>
@@ -823,7 +906,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,10 +1013,12 @@
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="3">
-        <v>14.1</v>
-      </c>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1188,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C57804-2851-444A-A2E0-BCB7B7087E9B}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,4 +1364,299 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B75042-AEB6-4CEB-B4DC-0578AD0E5FC4}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09B9B1F-2B0D-4B8D-9E08-46AF781AAA3A}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add deactivate option to explorer config
</commit_message>
<xml_diff>
--- a/QCA-AID-Explorer-Config.xlsx
+++ b/QCA-AID-Explorer-Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="11_AD4DB114E441178AC67DF462BE53C4D2693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA7D2BDA-EA5F-4648-B29C-A7BF310B1314}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="11_AD4DB114E441178AC67DF462BE53C4D2693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B46055EC-9DFB-49AA-8F67-ED751902DAF0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t>Parameter</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>Kritisch, Befürwortend, Ambivalent, Neutral</t>
-  </si>
-  <si>
-    <t>Sentiment-Analyse: Ressourcen (Kritisch/Befürwortend)</t>
   </si>
   <si>
     <t>Custom Prompt</t>
@@ -302,6 +299,18 @@
     "keywords": ["wort1", "wort2", "wort3"], // 3-5 Schlüsselwörter, die zur Bewertung von Ressourcen im Text entscheidend sind
     "explanation": "Kurze Begründung" // Kurze Erklärung (1-2 Sätze)
 }}</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zum deaktivieren der Auswertung hier "false" </t>
+  </si>
+  <si>
+    <t>Sentiment-Analyse: Rahmenbedingungen (Kritisch/Befürwortend)</t>
   </si>
 </sst>
 </file>
@@ -377,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,6 +398,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -782,17 +792,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEAB7FE-7933-4B3B-A453-4211109DE74F}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -806,93 +816,104 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="3">
+        <v>150</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -903,10 +924,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F11B677-61CF-43EB-A7F1-A53D79D62C9D}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,116 +948,127 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>73</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1045,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07585485-DB68-49AA-8D17-FBBBAA695720}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,83 +1101,89 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1166,6 +1204,11 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1174,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14C4134-1CFA-4F70-B278-210D6020E806}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,69 +1241,80 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1271,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C57804-2851-444A-A2E0-BCB7B7087E9B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,71 +1349,82 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1368,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B75042-AEB6-4CEB-B4DC-0578AD0E5FC4}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,115 +1458,126 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>79</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1510,9 +1586,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09B9B1F-2B0D-4B8D-9E08-46AF781AAA3A}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1535,126 +1611,137 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>